<commit_message>
Electives Replace in User Schedule
-Now using case with best match score to replace electives in schedule
-Added track button with functionality
</commit_message>
<xml_diff>
--- a/Cases.xlsx
+++ b/Cases.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Katie\Documents\GitHub\SmartClassPlanningTool\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D7DBA13-B39A-45E4-B254-3E01F02B734F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -142,9 +151,6 @@
     <t>CPSC 3105, CPSC 3165, CPSC 4121E, HIST 1111, GE, PEDS 1355</t>
   </si>
   <si>
-    <t>CPSC 4125, CPSC 4175, CPSC 4115, GE, GE</t>
-  </si>
-  <si>
     <t>CPSC 4176, CPSC 4126, CPSC 4135, CPSC 4000, CPSC 4145E, GE</t>
   </si>
   <si>
@@ -166,29 +172,33 @@
     <t>CPSC 3165, CYBR 3119, CYBR 4128, POLS 1101, Social Science GE</t>
   </si>
   <si>
-    <t>CPSC 4157, CPSC 4127, CPSC 4130, CPSC 2125</t>
-  </si>
-  <si>
-    <t>CYBR 4160, CYBR 4166, CPSC 4000, CPSC 4138, CPSC 3118</t>
+    <t>CPSC 4157, CPSC 4127, CPSC 4130, CPSC 2125, CYBR 3136E</t>
+  </si>
+  <si>
+    <t>CYBR 4160, CYBR 4166, CPSC 4000, CPSC 4138, CPSC 3118, CYBR 3126E</t>
+  </si>
+  <si>
+    <t>CPSC 4125, CPSC 4175, CPSC 4115, GE, GE, CPSC 3118E</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -199,45 +209,49 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -427,24 +441,29 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="14.13"/>
-    <col customWidth="1" min="2" max="2" width="44.5"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="44.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -452,31 +471,31 @@
         <v>1</v>
       </c>
       <c r="C1" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D1" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="E1" s="2">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="F1" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="G1" s="2">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="H1" s="2">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="I1" s="2">
-        <v>8.0</v>
-      </c>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -501,14 +520,16 @@
       <c r="H2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
       <c r="L2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -536,13 +557,13 @@
       <c r="I3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
       <c r="L3" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -570,11 +591,11 @@
       <c r="I4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -602,74 +623,74 @@
       <c r="I5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
       <c r="L5" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I6" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="I6" s="4" t="s">
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="D7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="4" t="s">
+      <c r="F7" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="G7" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="H7" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="I7" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="I2:K2"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>